<commit_message>
Mapping int-cpd to virt and ext-cpd
</commit_message>
<xml_diff>
--- a/documentation/missing-fields.xlsx
+++ b/documentation/missing-fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aasteele/Documents/nso/nfvo-tosca/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{310F531B-40F6-7A45-B010-6683E37647AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{6C5D2F7F-656C-6449-8E43-CD221009D990}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19000"/>
   </bookViews>
@@ -340,7 +340,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -689,8 +688,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1048,8 +1047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1069,47 +1068,47 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1139,7 +1138,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E16" t="s">
@@ -1152,7 +1151,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E18" t="s">
@@ -1160,7 +1159,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E19" t="s">
@@ -1168,7 +1167,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E20" t="s">
@@ -1176,7 +1175,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G21" t="s">
@@ -1184,7 +1183,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G22" t="s">
@@ -1195,7 +1194,7 @@
       <c r="B24" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E24" t="s">
@@ -1208,7 +1207,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C26" t="s">
@@ -1216,7 +1215,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C27" t="s">
@@ -1224,7 +1223,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C28" t="s">
@@ -1232,7 +1231,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C29" t="s">
@@ -1243,7 +1242,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C30" t="s">
@@ -1374,7 +1373,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B53" t="s">
@@ -1422,7 +1421,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D62" s="2" t="s">
+      <c r="D62" s="1" t="s">
         <v>56</v>
       </c>
       <c r="E62" t="s">
@@ -1430,7 +1429,7 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="1" t="s">
         <v>57</v>
       </c>
       <c r="C63" t="s">
@@ -1441,7 +1440,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C64" t="s">
@@ -1452,7 +1451,7 @@
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C65" t="s">

</xml_diff>

<commit_message>
Made flavor name mapping
</commit_message>
<xml_diff>
--- a/documentation/missing-fields.xlsx
+++ b/documentation/missing-fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aasteele/Documents/nso/nfvo-tosca/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{6C5D2F7F-656C-6449-8E43-CD221009D990}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{676A6DD5-3F8D-4641-B2B2-8452DAB1C19E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19000"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
   <si>
     <t>VNFD</t>
   </si>
@@ -70,12 +70,6 @@
     <t>layer-protocol</t>
   </si>
   <si>
-    <t>interface-id</t>
-  </si>
-  <si>
-    <t>management</t>
-  </si>
-  <si>
     <t>additional-sol1-parameters</t>
   </si>
   <si>
@@ -167,9 +161,6 @@
   </si>
   <si>
     <t>int-virtual-link-desc[]</t>
-  </si>
-  <si>
-    <t>populating old virtual-link-descriptor tags</t>
   </si>
   <si>
     <t>ext-cpd []</t>
@@ -1045,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1062,87 +1053,84 @@
     <col min="7" max="7" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D16" s="1" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D16" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="E16" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1159,51 +1147,51 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E19" t="s">
+      <c r="G19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E20" t="s">
+      <c r="G20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F21" s="1" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
         <v>19</v>
       </c>
-      <c r="G21" t="s">
+      <c r="D22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D25" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1221,40 +1209,40 @@
       <c r="C27" t="s">
         <v>14</v>
       </c>
+      <c r="D27" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
         <v>29</v>
       </c>
-      <c r="C30" t="s">
-        <v>14</v>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="B32" t="s">
         <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>1</v>
       </c>
       <c r="D32" t="s">
         <v>31</v>
@@ -1262,23 +1250,17 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>32</v>
       </c>
-      <c r="D34" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1302,25 +1284,25 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
+      <c r="A40" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>1</v>
-      </c>
-      <c r="D43" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1330,135 +1312,119 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
+      <c r="A45" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B50" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B51" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>48</v>
       </c>
-      <c r="B52" t="s">
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B53" t="s">
-        <v>28</v>
-      </c>
-    </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>51</v>
+      <c r="B54" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>52</v>
+      <c r="B55" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D57" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B57" t="s">
-        <v>11</v>
-      </c>
-    </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B58" t="s">
-        <v>53</v>
+      <c r="D58" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D59" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D60" t="s">
+      <c r="D60" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E60" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B61" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C61" t="s">
+        <v>14</v>
+      </c>
       <c r="D61" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B62" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D62" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E62" t="s">
+      <c r="C62" t="s">
         <v>14</v>
+      </c>
+      <c r="D62" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B63" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C63" t="s">
         <v>14</v>
       </c>
       <c r="D63" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B64" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C64" t="s">
-        <v>14</v>
-      </c>
-      <c r="D64" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B65" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C65" t="s">
-        <v>14</v>
-      </c>
-      <c r="D65" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Documentation, also don't save ~$ files
</commit_message>
<xml_diff>
--- a/documentation/missing-fields.xlsx
+++ b/documentation/missing-fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aasteele/Documents/nso/nfvo-tosca/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{676A6DD5-3F8D-4641-B2B2-8452DAB1C19E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{15176FCD-5E64-E74B-8EE6-1D45B5CF3F45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19000"/>
   </bookViews>
@@ -1038,8 +1038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Adding freezing, plus adding logging instead of prints, and removed Errors.py
</commit_message>
<xml_diff>
--- a/documentation/missing-fields.xlsx
+++ b/documentation/missing-fields.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aasteele/Documents/nso/nfvo-tosca/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{15176FCD-5E64-E74B-8EE6-1D45B5CF3F45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74DAB8B-0E82-6D49-9341-DDC028EBA706}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19000"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="missing-fields" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
   <si>
     <t>VNFD</t>
   </si>
@@ -109,13 +109,7 @@
     <t>sw-image-desc []</t>
   </si>
   <si>
-    <t>value need to change</t>
-  </si>
-  <si>
     <t>image-name-variable</t>
-  </si>
-  <si>
-    <t>we can always populate this field</t>
   </si>
   <si>
     <t>checksum</t>
@@ -193,7 +187,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -677,10 +671,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1035,11 +1030,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1166,11 +1161,8 @@
       <c r="B22" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="E22" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1179,27 +1171,18 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C24" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C25" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="C26" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1228,24 +1211,15 @@
       <c r="B30" t="s">
         <v>1</v>
       </c>
-      <c r="D30" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>10</v>
       </c>
-      <c r="D31" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>30</v>
-      </c>
-      <c r="D32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1255,37 +1229,37 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1293,27 +1267,27 @@
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1323,12 +1297,12 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -1338,22 +1312,22 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -1368,7 +1342,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -1378,36 +1352,30 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D58" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D59" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D60" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E60" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B61" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C61" t="s">
-        <v>14</v>
-      </c>
-      <c r="D61" t="s">
-        <v>26</v>
+      <c r="B61" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B62" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C62" t="s">
         <v>14</v>
@@ -1418,7 +1386,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B63" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C63" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Renaming main file to solcon from tosca
</commit_message>
<xml_diff>
--- a/documentation/missing-fields.xlsx
+++ b/documentation/missing-fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aasteele/Documents/nso/nfvo-tosca/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74DAB8B-0E82-6D49-9341-DDC028EBA706}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917374EB-4472-BC4D-99B3-6EFF6B5220A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1033,8 +1033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>